<commit_message>
adding hp to charactor
</commit_message>
<xml_diff>
--- a/hw1_score_s1061506.xlsx
+++ b/hw1_score_s1061506.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>坦克前後移動</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,6 +283,10 @@
   </si>
   <si>
     <t>按 Q 自動左轉，按 E 自動右轉，R 自動前進(靜止下可按 3 次達到最大前進速度)，F 自動後退(靜止下可按 3 次達到最大後退速度)，T 切換鏡頭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP = 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -733,7 +737,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="22.2" x14ac:dyDescent="0.3"/>
@@ -1047,7 +1051,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>61</v>
@@ -1078,8 +1082,12 @@
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="D28" s="1">
         <v>5</v>
       </c>

</xml_diff>